<commit_message>
Updates app to include backup data sourcing and request throttling to remain within API query limits.
</commit_message>
<xml_diff>
--- a/stock_forecasts_2025-05-02.xlsx
+++ b/stock_forecasts_2025-05-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sar81\stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACC046C-F568-44D1-B2F9-D60921EA57F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A317AFAA-9803-4987-982D-04A14C4B7B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="915" firstSheet="20" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19716,7 +19716,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>